<commit_message>
made id 8 digits
</commit_message>
<xml_diff>
--- a/assets/db-orig-and-updated.xlsx
+++ b/assets/db-orig-and-updated.xlsx
@@ -4935,7 +4935,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0000"/>
+    <numFmt numFmtId="165" formatCode="00000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -5743,7 +5743,7 @@
   <dimension ref="A1:G260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>